<commit_message>
Make preprocessing of data easier to manage
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\OneDrive - NTNU\Indok\9. semester\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\OneDrive - NTNU\Indok\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C3A3EB-F7E7-45DB-BA34-82742ECBC90C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{6A333D86-0EFE-48C5-877A-6581EBDEDD92}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Inflation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>PALUM</t>
   </si>
@@ -507,12 +507,6 @@
     <t>Zinc</t>
   </si>
   <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Inflation Index</t>
-  </si>
-  <si>
     <t>PALLFNF</t>
   </si>
   <si>
@@ -1066,7 +1060,7 @@
         <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:55" ht="148.19999999999999" x14ac:dyDescent="0.3">
@@ -1233,7 +1227,7 @@
         <v>106</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:55" ht="22.8" x14ac:dyDescent="0.3">
@@ -1398,7 +1392,7 @@
         <v>159</v>
       </c>
       <c r="BC3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.3">
@@ -46495,2191 +46489,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72859382-0657-47F6-BC2B-4A806A6E8CD7}">
-  <dimension ref="A1:B271"/>
-  <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>34700</v>
-      </c>
-      <c r="B2">
-        <v>0.61392809999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>34731</v>
-      </c>
-      <c r="B3">
-        <v>0.61775760000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>34759</v>
-      </c>
-      <c r="B4">
-        <v>0.62186019999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>34790</v>
-      </c>
-      <c r="B5">
-        <v>0.62706050000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>34820</v>
-      </c>
-      <c r="B6">
-        <v>0.63019380000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>34851</v>
-      </c>
-      <c r="B7">
-        <v>0.63240240000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>34881</v>
-      </c>
-      <c r="B8">
-        <v>0.63327840000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>34912</v>
-      </c>
-      <c r="B9">
-        <v>0.63592480000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>34943</v>
-      </c>
-      <c r="B10">
-        <v>0.63988460000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>34973</v>
-      </c>
-      <c r="B11">
-        <v>0.64261509999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>35004</v>
-      </c>
-      <c r="B12">
-        <v>0.64452110000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>35034</v>
-      </c>
-      <c r="B13">
-        <v>0.64707840000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>35065</v>
-      </c>
-      <c r="B14">
-        <v>0.65153949999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>35096</v>
-      </c>
-      <c r="B15">
-        <v>0.65463389999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>35125</v>
-      </c>
-      <c r="B16">
-        <v>0.65872829999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>35156</v>
-      </c>
-      <c r="B17">
-        <v>0.66299920000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>35186</v>
-      </c>
-      <c r="B18">
-        <v>0.66567569999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>35217</v>
-      </c>
-      <c r="B19">
-        <v>0.66676860000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>35247</v>
-      </c>
-      <c r="B20">
-        <v>0.66790159999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
-        <v>35278</v>
-      </c>
-      <c r="B21">
-        <v>0.66993320000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>35309</v>
-      </c>
-      <c r="B22">
-        <v>0.67340900000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>35339</v>
-      </c>
-      <c r="B23">
-        <v>0.67654610000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>35370</v>
-      </c>
-      <c r="B24">
-        <v>0.67861630000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>35400</v>
-      </c>
-      <c r="B25">
-        <v>0.68110420000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
-        <v>35431</v>
-      </c>
-      <c r="B26">
-        <v>0.68456050000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>35462</v>
-      </c>
-      <c r="B27">
-        <v>0.6871758</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>35490</v>
-      </c>
-      <c r="B28">
-        <v>0.68970719999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
-        <v>35521</v>
-      </c>
-      <c r="B29">
-        <v>0.69338160000000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
-        <v>35551</v>
-      </c>
-      <c r="B30">
-        <v>0.69511179999999995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
-        <v>35582</v>
-      </c>
-      <c r="B31">
-        <v>0.69670270000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
-        <v>35612</v>
-      </c>
-      <c r="B32">
-        <v>0.69855519999999993</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
-        <v>35643</v>
-      </c>
-      <c r="B33">
-        <v>0.70141949999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
-        <v>35674</v>
-      </c>
-      <c r="B34">
-        <v>0.70524389999999992</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
-        <v>35704</v>
-      </c>
-      <c r="B35">
-        <v>0.70862759999999991</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
-        <v>35735</v>
-      </c>
-      <c r="B36">
-        <v>0.71035359999999992</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
-        <v>35765</v>
-      </c>
-      <c r="B37">
-        <v>0.71250079999999993</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
-        <v>35796</v>
-      </c>
-      <c r="B38">
-        <v>0.71547369999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>35827</v>
-      </c>
-      <c r="B39">
-        <v>0.7182037</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>35855</v>
-      </c>
-      <c r="B40">
-        <v>0.72065219999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
-        <v>35886</v>
-      </c>
-      <c r="B41">
-        <v>0.72337950000000006</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
-        <v>35916</v>
-      </c>
-      <c r="B42">
-        <v>0.72547510000000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <v>35947</v>
-      </c>
-      <c r="B43">
-        <v>0.72640760000000004</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
-        <v>35977</v>
-      </c>
-      <c r="B44">
-        <v>0.72719449999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
-        <v>36008</v>
-      </c>
-      <c r="B45">
-        <v>0.72860140000000007</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>36039</v>
-      </c>
-      <c r="B46">
-        <v>0.73189400000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
-        <v>36069</v>
-      </c>
-      <c r="B47">
-        <v>0.73532459999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
-        <v>36100</v>
-      </c>
-      <c r="B48">
-        <v>0.73686499999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
-        <v>36130</v>
-      </c>
-      <c r="B49">
-        <v>0.73819480000000004</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
-        <v>36161</v>
-      </c>
-      <c r="B50">
-        <v>0.73990610000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
-        <v>36192</v>
-      </c>
-      <c r="B51">
-        <v>0.7414828</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
-        <v>36220</v>
-      </c>
-      <c r="B52">
-        <v>0.74449579999999993</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
-        <v>36251</v>
-      </c>
-      <c r="B53">
-        <v>0.74942570000000008</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
-        <v>36281</v>
-      </c>
-      <c r="B54">
-        <v>0.75049929999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
-        <v>36312</v>
-      </c>
-      <c r="B55">
-        <v>0.75107889999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
-        <v>36342</v>
-      </c>
-      <c r="B56">
-        <v>0.7528355000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
-        <v>36373</v>
-      </c>
-      <c r="B57">
-        <v>0.75543719999999992</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
-        <v>36404</v>
-      </c>
-      <c r="B58">
-        <v>0.75942319999999996</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4">
-        <v>36434</v>
-      </c>
-      <c r="B59">
-        <v>0.76226330000000009</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
-        <v>36465</v>
-      </c>
-      <c r="B60">
-        <v>0.76373210000000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="4">
-        <v>36495</v>
-      </c>
-      <c r="B61">
-        <v>0.76620130000000009</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
-        <v>36526</v>
-      </c>
-      <c r="B62">
-        <v>0.76840790000000003</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
-        <v>36557</v>
-      </c>
-      <c r="B63">
-        <v>0.77194640000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
-        <v>36586</v>
-      </c>
-      <c r="B64">
-        <v>0.77651290000000006</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
-        <v>36617</v>
-      </c>
-      <c r="B65">
-        <v>0.77793229999999991</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
-        <v>36647</v>
-      </c>
-      <c r="B66">
-        <v>0.77948499999999998</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="4">
-        <v>36678</v>
-      </c>
-      <c r="B67">
-        <v>0.78238829999999993</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
-        <v>36708</v>
-      </c>
-      <c r="B68">
-        <v>0.78432060000000003</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
-        <v>36739</v>
-      </c>
-      <c r="B69">
-        <v>0.78528989999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
-        <v>36770</v>
-      </c>
-      <c r="B70">
-        <v>0.78945009999999993</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
-        <v>36800</v>
-      </c>
-      <c r="B71">
-        <v>0.79129070000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
-        <v>36831</v>
-      </c>
-      <c r="B72">
-        <v>0.79286979999999996</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
-        <v>36861</v>
-      </c>
-      <c r="B73">
-        <v>0.79427159999999997</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="4">
-        <v>36892</v>
-      </c>
-      <c r="B74">
-        <v>0.79679689999999992</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="4">
-        <v>36923</v>
-      </c>
-      <c r="B75">
-        <v>0.79942729999999995</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4">
-        <v>36951</v>
-      </c>
-      <c r="B76">
-        <v>0.8024903000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="4">
-        <v>36982</v>
-      </c>
-      <c r="B77">
-        <v>0.80788799999999994</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="4">
-        <v>37012</v>
-      </c>
-      <c r="B78">
-        <v>0.81223630000000002</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="4">
-        <v>37043</v>
-      </c>
-      <c r="B79">
-        <v>0.81376850000000001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="4">
-        <v>37073</v>
-      </c>
-      <c r="B80">
-        <v>0.81265180000000004</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="4">
-        <v>37104</v>
-      </c>
-      <c r="B81">
-        <v>0.81396370000000007</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="4">
-        <v>37135</v>
-      </c>
-      <c r="B82">
-        <v>0.81758970000000009</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="4">
-        <v>37165</v>
-      </c>
-      <c r="B83">
-        <v>0.81807829999999992</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="4">
-        <v>37196</v>
-      </c>
-      <c r="B84">
-        <v>0.81778499999999998</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="4">
-        <v>37226</v>
-      </c>
-      <c r="B85">
-        <v>0.8183359</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="4">
-        <v>37257</v>
-      </c>
-      <c r="B86">
-        <v>0.82100010000000001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="4">
-        <v>37288</v>
-      </c>
-      <c r="B87">
-        <v>0.82306060000000003</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="4">
-        <v>37316</v>
-      </c>
-      <c r="B88">
-        <v>0.827075</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="4">
-        <v>37347</v>
-      </c>
-      <c r="B89">
-        <v>0.83127589999999996</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="4">
-        <v>37377</v>
-      </c>
-      <c r="B90">
-        <v>0.8324028</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="4">
-        <v>37408</v>
-      </c>
-      <c r="B91">
-        <v>0.83270669999999991</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="4">
-        <v>37438</v>
-      </c>
-      <c r="B92">
-        <v>0.83293629999999996</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="4">
-        <v>37469</v>
-      </c>
-      <c r="B93">
-        <v>0.83535579999999998</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="4">
-        <v>37500</v>
-      </c>
-      <c r="B94">
-        <v>0.83770230000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="4">
-        <v>37530</v>
-      </c>
-      <c r="B95">
-        <v>0.83964420000000006</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="4">
-        <v>37561</v>
-      </c>
-      <c r="B96">
-        <v>0.84045190000000003</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="4">
-        <v>37591</v>
-      </c>
-      <c r="B97">
-        <v>0.84121290000000004</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="4">
-        <v>37622</v>
-      </c>
-      <c r="B98">
-        <v>0.84376700000000004</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="4">
-        <v>37653</v>
-      </c>
-      <c r="B99">
-        <v>0.84812830000000006</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="4">
-        <v>37681</v>
-      </c>
-      <c r="B100">
-        <v>0.85257149999999993</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="4">
-        <v>37712</v>
-      </c>
-      <c r="B101">
-        <v>0.85230860000000008</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="4">
-        <v>37742</v>
-      </c>
-      <c r="B102">
-        <v>0.85181870000000004</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="4">
-        <v>37773</v>
-      </c>
-      <c r="B103">
-        <v>0.85212639999999995</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="4">
-        <v>37803</v>
-      </c>
-      <c r="B104">
-        <v>0.85204520000000006</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="4">
-        <v>37834</v>
-      </c>
-      <c r="B105">
-        <v>0.85440830000000001</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="4">
-        <v>37865</v>
-      </c>
-      <c r="B106">
-        <v>0.85719020000000001</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="4">
-        <v>37895</v>
-      </c>
-      <c r="B107">
-        <v>0.85762369999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="4">
-        <v>37926</v>
-      </c>
-      <c r="B108">
-        <v>0.85691130000000004</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="4">
-        <v>37956</v>
-      </c>
-      <c r="B109">
-        <v>0.85775170000000001</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="4">
-        <v>37987</v>
-      </c>
-      <c r="B110">
-        <v>0.85969960000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="4">
-        <v>38018</v>
-      </c>
-      <c r="B111">
-        <v>0.86279300000000003</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="4">
-        <v>38047</v>
-      </c>
-      <c r="B112">
-        <v>0.86705830000000006</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="4">
-        <v>38078</v>
-      </c>
-      <c r="B113">
-        <v>0.86983549999999998</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="4">
-        <v>38108</v>
-      </c>
-      <c r="B114">
-        <v>0.87331340000000002</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="4">
-        <v>38139</v>
-      </c>
-      <c r="B115">
-        <v>0.87486929999999996</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="4">
-        <v>38169</v>
-      </c>
-      <c r="B116">
-        <v>0.87391819999999998</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="4">
-        <v>38200</v>
-      </c>
-      <c r="B117">
-        <v>0.87519610000000003</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="4">
-        <v>38231</v>
-      </c>
-      <c r="B118">
-        <v>0.87703819999999988</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="4">
-        <v>38261</v>
-      </c>
-      <c r="B119">
-        <v>0.88113960000000002</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="4">
-        <v>38292</v>
-      </c>
-      <c r="B120">
-        <v>0.88169809999999993</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="4">
-        <v>38322</v>
-      </c>
-      <c r="B121">
-        <v>0.88104179999999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4">
-        <v>38353</v>
-      </c>
-      <c r="B122">
-        <v>0.88084560000000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="4">
-        <v>38384</v>
-      </c>
-      <c r="B123">
-        <v>0.88405540000000005</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="4">
-        <v>38412</v>
-      </c>
-      <c r="B124">
-        <v>0.88922630000000003</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="4">
-        <v>38443</v>
-      </c>
-      <c r="B125">
-        <v>0.89323549999999996</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="4">
-        <v>38473</v>
-      </c>
-      <c r="B126">
-        <v>0.89373410000000009</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="4">
-        <v>38504</v>
-      </c>
-      <c r="B127">
-        <v>0.89376949999999988</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="4">
-        <v>38534</v>
-      </c>
-      <c r="B128">
-        <v>0.89590500000000006</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="4">
-        <v>38565</v>
-      </c>
-      <c r="B129">
-        <v>0.89886560000000004</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="4">
-        <v>38596</v>
-      </c>
-      <c r="B130">
-        <v>0.90543289999999998</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="4">
-        <v>38626</v>
-      </c>
-      <c r="B131">
-        <v>0.90729490000000002</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="4">
-        <v>38657</v>
-      </c>
-      <c r="B132">
-        <v>0.90394839999999999</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="4">
-        <v>38687</v>
-      </c>
-      <c r="B133">
-        <v>0.90352199999999994</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="4">
-        <v>38718</v>
-      </c>
-      <c r="B134">
-        <v>0.90664800000000001</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="4">
-        <v>38749</v>
-      </c>
-      <c r="B135">
-        <v>0.90821299999999994</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="4">
-        <v>38777</v>
-      </c>
-      <c r="B136">
-        <v>0.91182280000000004</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="4">
-        <v>38808</v>
-      </c>
-      <c r="B137">
-        <v>0.91780269999999997</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="4">
-        <v>38838</v>
-      </c>
-      <c r="B138">
-        <v>0.92137119999999995</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="4">
-        <v>38869</v>
-      </c>
-      <c r="B139">
-        <v>0.92244470000000012</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="4">
-        <v>38899</v>
-      </c>
-      <c r="B140">
-        <v>0.92387510000000006</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="4">
-        <v>38930</v>
-      </c>
-      <c r="B141">
-        <v>0.92608120000000005</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="4">
-        <v>38961</v>
-      </c>
-      <c r="B142">
-        <v>0.92472969999999999</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="4">
-        <v>38991</v>
-      </c>
-      <c r="B143">
-        <v>0.92278530000000003</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="4">
-        <v>39022</v>
-      </c>
-      <c r="B144">
-        <v>0.92249629999999994</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="4">
-        <v>39052</v>
-      </c>
-      <c r="B145">
-        <v>0.92457250000000002</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="4">
-        <v>39083</v>
-      </c>
-      <c r="B146">
-        <v>0.92523460000000002</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="4">
-        <v>39114</v>
-      </c>
-      <c r="B147">
-        <v>0.92836889999999994</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="4">
-        <v>39142</v>
-      </c>
-      <c r="B148">
-        <v>0.93431500000000001</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="4">
-        <v>39173</v>
-      </c>
-      <c r="B149">
-        <v>0.93948359999999997</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="4">
-        <v>39203</v>
-      </c>
-      <c r="B150">
-        <v>0.94288629999999996</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="4">
-        <v>39234</v>
-      </c>
-      <c r="B151">
-        <v>0.94383870000000003</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="4">
-        <v>39264</v>
-      </c>
-      <c r="B152">
-        <v>0.94359459999999995</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="4">
-        <v>39295</v>
-      </c>
-      <c r="B153">
-        <v>0.94382650000000001</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="4">
-        <v>39326</v>
-      </c>
-      <c r="B154">
-        <v>0.94654459999999996</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="4">
-        <v>39356</v>
-      </c>
-      <c r="B155">
-        <v>0.94986630000000005</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="4">
-        <v>39387</v>
-      </c>
-      <c r="B156">
-        <v>0.95448580000000005</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="4">
-        <v>39417</v>
-      </c>
-      <c r="B157">
-        <v>0.95612459999999999</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="4">
-        <v>39448</v>
-      </c>
-      <c r="B158">
-        <v>0.95822399999999996</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="4">
-        <v>39479</v>
-      </c>
-      <c r="B159">
-        <v>0.96107900000000002</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="4">
-        <v>39508</v>
-      </c>
-      <c r="B160">
-        <v>0.96804029999999996</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="4">
-        <v>39539</v>
-      </c>
-      <c r="B161">
-        <v>0.97279210000000005</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="4">
-        <v>39569</v>
-      </c>
-      <c r="B162">
-        <v>0.97980549999999988</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="4">
-        <v>39600</v>
-      </c>
-      <c r="B163">
-        <v>0.98605799999999999</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="4">
-        <v>39630</v>
-      </c>
-      <c r="B164">
-        <v>0.98963359999999989</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="4">
-        <v>39661</v>
-      </c>
-      <c r="B165">
-        <v>0.98843119999999995</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="4">
-        <v>39692</v>
-      </c>
-      <c r="B166">
-        <v>0.98889250000000006</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="4">
-        <v>39722</v>
-      </c>
-      <c r="B167">
-        <v>0.98511759999999993</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="4">
-        <v>39753</v>
-      </c>
-      <c r="B168">
-        <v>0.97582290000000005</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="4">
-        <v>39783</v>
-      </c>
-      <c r="B169">
-        <v>0.97055210000000003</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="4">
-        <v>39814</v>
-      </c>
-      <c r="B170">
-        <v>0.97038820000000003</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="4">
-        <v>39845</v>
-      </c>
-      <c r="B171">
-        <v>0.97390080000000001</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="4">
-        <v>39873</v>
-      </c>
-      <c r="B172">
-        <v>0.97652530000000004</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="4">
-        <v>39904</v>
-      </c>
-      <c r="B173">
-        <v>0.97888580000000003</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="4">
-        <v>39934</v>
-      </c>
-      <c r="B174">
-        <v>0.98060820000000004</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="4">
-        <v>39965</v>
-      </c>
-      <c r="B175">
-        <v>0.98473549999999999</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="4">
-        <v>39995</v>
-      </c>
-      <c r="B176">
-        <v>0.98334140000000003</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="4">
-        <v>40026</v>
-      </c>
-      <c r="B177">
-        <v>0.98539510000000008</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="4">
-        <v>40057</v>
-      </c>
-      <c r="B178">
-        <v>0.98585199999999995</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="4">
-        <v>40087</v>
-      </c>
-      <c r="B179">
-        <v>0.98702610000000002</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="4">
-        <v>40118</v>
-      </c>
-      <c r="B180">
-        <v>0.98835200000000001</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="4">
-        <v>40148</v>
-      </c>
-      <c r="B181">
-        <v>0.98872539999999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="4">
-        <v>40179</v>
-      </c>
-      <c r="B182">
-        <v>0.99072590000000005</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="4">
-        <v>40210</v>
-      </c>
-      <c r="B183">
-        <v>0.99265349999999997</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="4">
-        <v>40238</v>
-      </c>
-      <c r="B184">
-        <v>0.99700940000000005</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="4">
-        <v>40269</v>
-      </c>
-      <c r="B185">
-        <v>0.99968410000000008</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="4">
-        <v>40299</v>
-      </c>
-      <c r="B186">
-        <v>1.0001229999999999</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="4">
-        <v>40330</v>
-      </c>
-      <c r="B187">
-        <v>0.99940280000000004</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="4">
-        <v>40360</v>
-      </c>
-      <c r="B188">
-        <v>0.99907259999999998</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="4">
-        <v>40391</v>
-      </c>
-      <c r="B189">
-        <v>1.0006090000000001</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="4">
-        <v>40422</v>
-      </c>
-      <c r="B190">
-        <v>1.0021659999999999</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="4">
-        <v>40452</v>
-      </c>
-      <c r="B191">
-        <v>1.004834</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="4">
-        <v>40483</v>
-      </c>
-      <c r="B192">
-        <v>1.005538</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="4">
-        <v>40513</v>
-      </c>
-      <c r="B193">
-        <v>1.0081829999999998</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="4">
-        <v>40544</v>
-      </c>
-      <c r="B194">
-        <v>1.011072</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="4">
-        <v>40575</v>
-      </c>
-      <c r="B195">
-        <v>1.0152870000000001</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="4">
-        <v>40603</v>
-      </c>
-      <c r="B196">
-        <v>1.0225629999999999</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="4">
-        <v>40634</v>
-      </c>
-      <c r="B197">
-        <v>1.0278560000000001</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="4">
-        <v>40664</v>
-      </c>
-      <c r="B198">
-        <v>1.03077</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="4">
-        <v>40695</v>
-      </c>
-      <c r="B199">
-        <v>1.02956</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="4">
-        <v>40725</v>
-      </c>
-      <c r="B200">
-        <v>1.0299659999999999</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="4">
-        <v>40756</v>
-      </c>
-      <c r="B201">
-        <v>1.0324230000000001</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="4">
-        <v>40787</v>
-      </c>
-      <c r="B202">
-        <v>1.034538</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="4">
-        <v>40817</v>
-      </c>
-      <c r="B203">
-        <v>1.035962</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="4">
-        <v>40848</v>
-      </c>
-      <c r="B204">
-        <v>1.0366230000000001</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="4">
-        <v>40878</v>
-      </c>
-      <c r="B205">
-        <v>1.0371060000000001</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="4">
-        <v>40909</v>
-      </c>
-      <c r="B206">
-        <v>1.039412</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="4">
-        <v>40940</v>
-      </c>
-      <c r="B207">
-        <v>1.0435970000000001</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="4">
-        <v>40969</v>
-      </c>
-      <c r="B208">
-        <v>1.049731</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="4">
-        <v>41000</v>
-      </c>
-      <c r="B209">
-        <v>1.053021</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="4">
-        <v>41030</v>
-      </c>
-      <c r="B210">
-        <v>1.051892</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="4">
-        <v>41061</v>
-      </c>
-      <c r="B211">
-        <v>1.050038</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="4">
-        <v>41091</v>
-      </c>
-      <c r="B212">
-        <v>1.0492589999999999</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="4">
-        <v>41122</v>
-      </c>
-      <c r="B213">
-        <v>1.05359</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="4">
-        <v>41153</v>
-      </c>
-      <c r="B214">
-        <v>1.0574060000000001</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="4">
-        <v>41183</v>
-      </c>
-      <c r="B215">
-        <v>1.059094</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="4">
-        <v>41214</v>
-      </c>
-      <c r="B216">
-        <v>1.056727</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="4">
-        <v>41244</v>
-      </c>
-      <c r="B217">
-        <v>1.0564069999999999</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="4">
-        <v>41275</v>
-      </c>
-      <c r="B218">
-        <v>1.0573680000000001</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="4">
-        <v>41306</v>
-      </c>
-      <c r="B219">
-        <v>1.062697</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="4">
-        <v>41334</v>
-      </c>
-      <c r="B220">
-        <v>1.066346</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="4">
-        <v>41365</v>
-      </c>
-      <c r="B221">
-        <v>1.0663100000000001</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="4">
-        <v>41395</v>
-      </c>
-      <c r="B222">
-        <v>1.067658</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="4">
-        <v>41426</v>
-      </c>
-      <c r="B223">
-        <v>1.0691459999999999</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="4">
-        <v>41456</v>
-      </c>
-      <c r="B224">
-        <v>1.070025</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="4">
-        <v>41487</v>
-      </c>
-      <c r="B225">
-        <v>1.0715519999999998</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="4">
-        <v>41518</v>
-      </c>
-      <c r="B226">
-        <v>1.0732360000000001</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="4">
-        <v>41548</v>
-      </c>
-      <c r="B227">
-        <v>1.072838</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="4">
-        <v>41579</v>
-      </c>
-      <c r="B228">
-        <v>1.0723590000000001</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="4">
-        <v>41609</v>
-      </c>
-      <c r="B229">
-        <v>1.073793</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="4">
-        <v>41640</v>
-      </c>
-      <c r="B230">
-        <v>1.0749250000000001</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="4">
-        <v>41671</v>
-      </c>
-      <c r="B231">
-        <v>1.078101</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="4">
-        <v>41699</v>
-      </c>
-      <c r="B232">
-        <v>1.0832189999999999</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="4">
-        <v>41730</v>
-      </c>
-      <c r="B233">
-        <v>1.0880529999999999</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="4">
-        <v>41760</v>
-      </c>
-      <c r="B234">
-        <v>1.090001</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="4">
-        <v>41791</v>
-      </c>
-      <c r="B235">
-        <v>1.0912839999999999</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="4">
-        <v>41821</v>
-      </c>
-      <c r="B236">
-        <v>1.0910599999999999</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="4">
-        <v>41852</v>
-      </c>
-      <c r="B237">
-        <v>1.0909659999999999</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="4">
-        <v>41883</v>
-      </c>
-      <c r="B238">
-        <v>1.0919459999999999</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="4">
-        <v>41913</v>
-      </c>
-      <c r="B239">
-        <v>1.0915189999999999</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="4">
-        <v>41944</v>
-      </c>
-      <c r="B240">
-        <v>1.0883499999999999</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="4">
-        <v>41974</v>
-      </c>
-      <c r="B241">
-        <v>1.0854280000000001</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="4">
-        <v>42005</v>
-      </c>
-      <c r="B242">
-        <v>1.080703</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="4">
-        <v>42036</v>
-      </c>
-      <c r="B243">
-        <v>1.0844940000000001</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="4">
-        <v>42064</v>
-      </c>
-      <c r="B244">
-        <v>1.0900080000000001</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="4">
-        <v>42095</v>
-      </c>
-      <c r="B245">
-        <v>1.092919</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="4">
-        <v>42125</v>
-      </c>
-      <c r="B246">
-        <v>1.0962909999999999</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="4">
-        <v>42156</v>
-      </c>
-      <c r="B247">
-        <v>1.0978250000000001</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="4">
-        <v>42186</v>
-      </c>
-      <c r="B248">
-        <v>1.0973820000000001</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="4">
-        <v>42217</v>
-      </c>
-      <c r="B249">
-        <v>1.09724</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="4">
-        <v>42248</v>
-      </c>
-      <c r="B250">
-        <v>1.096508</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="4">
-        <v>42278</v>
-      </c>
-      <c r="B251">
-        <v>1.0975539999999999</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="4">
-        <v>42309</v>
-      </c>
-      <c r="B252">
-        <v>1.0964260000000001</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="4">
-        <v>42339</v>
-      </c>
-      <c r="B253">
-        <v>1.0948169999999999</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="4">
-        <v>42370</v>
-      </c>
-      <c r="B254">
-        <v>1.093343</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="4">
-        <v>42401</v>
-      </c>
-      <c r="B255">
-        <v>1.0947280000000001</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="4">
-        <v>42430</v>
-      </c>
-      <c r="B256">
-        <v>1.0989990000000001</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="4">
-        <v>42461</v>
-      </c>
-      <c r="B257">
-        <v>1.1020159999999999</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="4">
-        <v>42491</v>
-      </c>
-      <c r="B258">
-        <v>1.105113</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="4">
-        <v>42522</v>
-      </c>
-      <c r="B259">
-        <v>1.1074630000000001</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="4">
-        <v>42552</v>
-      </c>
-      <c r="B260">
-        <v>1.106733</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="4">
-        <v>42583</v>
-      </c>
-      <c r="B261">
-        <v>1.1075980000000001</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="4">
-        <v>42614</v>
-      </c>
-      <c r="B262">
-        <v>1.109502</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="4">
-        <v>42644</v>
-      </c>
-      <c r="B263">
-        <v>1.112603</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="4">
-        <v>42675</v>
-      </c>
-      <c r="B264">
-        <v>1.1124049999999999</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="4">
-        <v>42705</v>
-      </c>
-      <c r="B265">
-        <v>1.114722</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="4">
-        <v>42736</v>
-      </c>
-      <c r="B266">
-        <v>1.11866</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="4">
-        <v>42767</v>
-      </c>
-      <c r="B267">
-        <v>1.1220969999999999</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="4">
-        <v>42795</v>
-      </c>
-      <c r="B268">
-        <v>1.1244050000000001</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="4">
-        <v>42826</v>
-      </c>
-      <c r="B269">
-        <v>1.128037</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="4">
-        <v>42856</v>
-      </c>
-      <c r="B270">
-        <v>1.1286799999999999</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="4">
-        <v>42887</v>
-      </c>
-      <c r="B271">
-        <v>1.128851</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>